<commit_message>
Reg Kiosk Backup (Commit Conflict)
</commit_message>
<xml_diff>
--- a/Timesheets/kjohnson4.xlsx
+++ b/Timesheets/kjohnson4.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Senior Project - Spring / Summer 2015</t>
   </si>
@@ -46,7 +46,25 @@
     <t>05/11/2015 Mon</t>
   </si>
   <si>
-    <t>12:30pm-</t>
+    <t>12:30pm-3:30pm</t>
+  </si>
+  <si>
+    <t>Minor Changes to GUI, Code Review, Class Meeting, Team Meeting</t>
+  </si>
+  <si>
+    <t>05/14/2015 Thu</t>
+  </si>
+  <si>
+    <t>5:45pm-9:45pm</t>
+  </si>
+  <si>
+    <t>Search Box Formatting, Hash Function, Additional GUI Work, Code Cleanup</t>
+  </si>
+  <si>
+    <t>05/15/2015 Fri</t>
+  </si>
+  <si>
+    <t>12:00pm-</t>
   </si>
 </sst>
 </file>
@@ -218,7 +236,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -227,7 +245,7 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.7091836734694"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.5714285714286"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.5765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="53.1428571428572"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="68.8265306122449"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
   </cols>
   <sheetData>
@@ -280,18 +298,34 @@
       <c r="C6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="D6" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
     </row>

</xml_diff>

<commit_message>
GUI Update (Add, Remove, and Edit working!)
</commit_message>
<xml_diff>
--- a/Timesheets/kjohnson4.xlsx
+++ b/Timesheets/kjohnson4.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Senior Project - Spring / Summer 2015</t>
   </si>
@@ -64,7 +64,10 @@
     <t>05/15/2015 Fri</t>
   </si>
   <si>
-    <t>12:00pm-</t>
+    <t>12:00pm-5:15pm</t>
+  </si>
+  <si>
+    <t>Fix Commit Conflict, Implement Database Functionality to GUI</t>
   </si>
 </sst>
 </file>
@@ -236,7 +239,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -326,8 +329,12 @@
       <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="D8" s="6" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>

</xml_diff>